<commit_message>
Style updated, mistake corrected
</commit_message>
<xml_diff>
--- a/PaediatricDosage.xlsx
+++ b/PaediatricDosage.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="409">
   <si>
     <t>Fluid  Requirement</t>
   </si>
@@ -1521,12 +1521,15 @@
     <t>Amoxicillin +
 Clavulinic acid</t>
   </si>
+  <si>
+    <t>Paracetamol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1577,6 +1580,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1598,7 +1615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1628,61 +1645,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1695,6 +1664,82 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1977,7 +2022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
@@ -1989,148 +2034,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="19">
         <v>60</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="19">
         <v>80</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="19">
         <v>100</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="19">
         <v>120</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="19">
         <v>140</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="19">
         <v>150</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="19"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="18"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
@@ -2196,21 +2241,21 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
@@ -2246,24 +2291,14 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="A17:B18"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="A33:C33"/>
@@ -2272,6 +2307,16 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2282,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView windowProtection="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2297,60 +2342,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="12"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="19"/>
+      <c r="A12" s="24"/>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
@@ -2406,42 +2451,42 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="25" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="15"/>
+      <c r="A22" s="25"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="41"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="13"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="40"/>
+      <c r="B24" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="43" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2449,29 +2494,29 @@
       <c r="A25" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:C5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:C8"/>
-    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:C8"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2482,9 +2527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2499,161 +2544,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="24"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="23"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.9" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="26"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45.95" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="36">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="23.65" customHeight="1">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" ht="48">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:6" ht="60">
+      <c r="A10" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="27" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B11" s="29" t="s">
@@ -2661,77 +2706,67 @@
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="182.25" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="24">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="26"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="23" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="25"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="B7:D7"/>
@@ -2740,6 +2775,16 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2751,8 +2796,8 @@
   <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2767,256 +2812,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="24"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="23"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.9" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="12" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45.95" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="26" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="24">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="27" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="61.5" customHeight="1">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="27" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:6" ht="72">
+      <c r="A11" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="12" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="63" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="26" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="26"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="45" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="24">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="31" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="14" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="12" t="s">
         <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
@@ -3025,11 +3070,11 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3041,8 +3086,8 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3057,317 +3102,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="24"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="23"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.9" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="12" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="32" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:6" ht="36">
+      <c r="A10" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="12" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="47.25" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="27" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="12" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="25" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="12" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="12" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="45" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F17" s="28"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="24">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="28"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="24">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27" t="s">
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="11" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="24">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
@@ -3376,6 +3411,16 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3387,13 +3432,13 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:D7"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="10" customWidth="1"/>
     <col min="3" max="3" width="13" style="10"/>
     <col min="4" max="4" width="13.42578125" style="10" customWidth="1"/>
@@ -3403,387 +3448,387 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="24"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="23"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.9" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="25" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="12" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="27" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="11" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="25" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="11" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45.95" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="47.25" customHeight="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="23"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="35"/>
+      <c r="B11" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="25" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="11" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F13" s="26"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="60" customHeight="1">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="25" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="11" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="12" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="12" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="27" t="s">
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="F18" s="28"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="24"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25" t="s">
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="72">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:6" ht="96">
+      <c r="A24" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="25" t="s">
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="12" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="25" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="11" t="s">
         <v>262</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:D23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A19:F21"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A9:F9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A19:F21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:D23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3796,12 +3841,12 @@
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="10" customWidth="1"/>
     <col min="2" max="3" width="10" style="10"/>
     <col min="4" max="4" width="13.42578125" style="10" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="10"/>
@@ -3810,314 +3855,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="11" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="11" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="30" t="s">
         <v>271</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" ht="6" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="25" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="12" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="49.5" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="25" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="36.75" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="26" t="s">
         <v>280</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="50.25" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="27" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="12" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F15" s="28"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="25" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="11" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27" t="s">
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="12" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="28" t="s">
         <v>297</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="28" t="s">
         <v>299</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="25" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="11" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60.75" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="27" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="87.75" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="25" t="s">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="12" t="s">
         <v>307</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A6:F8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B16:D16"/>
@@ -4125,6 +4155,21 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A6:F8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -4137,7 +4182,7 @@
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4150,19 +4195,19 @@
     <col min="7" max="1025" width="10" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="13.9" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:1024" ht="17.25" customHeight="1">
+      <c r="A1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="32"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -5183,20 +5228,20 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="22"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="33" t="s">
         <v>73</v>
       </c>
       <c r="G2"/>
@@ -6218,19 +6263,19 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" ht="49.5" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>349</v>
-      </c>
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="1:1024" ht="37.5" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="12" t="s">
         <v>310</v>
       </c>
       <c r="G3"/>
@@ -7252,19 +7297,19 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" ht="45" customHeight="1">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:1024" ht="37.5" customHeight="1">
+      <c r="A4" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="12" t="s">
         <v>314</v>
       </c>
       <c r="G4"/>
@@ -8287,18 +8332,18 @@
       <c r="AMJ4"/>
     </row>
     <row r="5" spans="1:1024" ht="32.25" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="27" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="11" t="s">
         <v>318</v>
       </c>
       <c r="G5"/>
@@ -9320,19 +9365,19 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024" ht="95.25" customHeight="1">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:1024" ht="64.5" customHeight="1">
+      <c r="A6" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="13"/>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
@@ -10353,16 +10398,16 @@
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="25" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="11" t="s">
         <v>73</v>
       </c>
       <c r="G7"/>
@@ -11384,19 +11429,19 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" ht="37.5" customHeight="1">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:1024" ht="26.25" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="12" t="s">
         <v>327</v>
       </c>
       <c r="G8"/>
@@ -12419,18 +12464,18 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" ht="24">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="13"/>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -13450,19 +13495,19 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" ht="60.75" customHeight="1">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:1024" ht="49.5" customHeight="1">
+      <c r="A10" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="25" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="11" t="s">
         <v>334</v>
       </c>
       <c r="G10"/>
@@ -14484,17 +14529,17 @@
       <c r="AMI10"/>
       <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1024" ht="35.25" customHeight="1">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:1024" ht="26.25" customHeight="1">
+      <c r="A11" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="25" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11" t="s">
         <v>337</v>
       </c>
       <c r="G11"/>
@@ -15516,17 +15561,17 @@
       <c r="AMI11"/>
       <c r="AMJ11"/>
     </row>
-    <row r="12" spans="1:1024" ht="43.5" customHeight="1">
-      <c r="A12" s="27" t="s">
+    <row r="12" spans="1:1024" ht="37.5" customHeight="1">
+      <c r="A12" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="25" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11" t="s">
         <v>340</v>
       </c>
       <c r="G12"/>
@@ -16548,19 +16593,19 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024" ht="45" customHeight="1">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:1024" ht="15.75" customHeight="1">
+      <c r="A13" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="25" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="11" t="s">
         <v>343</v>
       </c>
       <c r="G13"/>
@@ -17583,16 +17628,16 @@
       <c r="AMJ13"/>
     </row>
     <row r="14" spans="1:1024">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="28" t="s">
         <v>345</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="25" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11" t="s">
         <v>346</v>
       </c>
       <c r="G14"/>
@@ -18614,105 +18659,105 @@
       <c r="AMI14"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024" ht="31.5" customHeight="1">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:1024" ht="26.25" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:1024">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="28" t="s">
         <v>351</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="11" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A20" s="25" t="s">
+    <row r="20" spans="1:6" ht="39" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -18724,8 +18769,8 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18738,19 +18783,19 @@
     <col min="7" max="1025" width="10" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="13.9" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:1024" ht="17.25" customHeight="1">
+      <c r="A1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="32"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -19771,20 +19816,20 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="22"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="33" t="s">
         <v>73</v>
       </c>
       <c r="G2"/>
@@ -20807,16 +20852,16 @@
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" ht="25.35" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
@@ -21837,18 +21882,18 @@
       <c r="AMJ3"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>364</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="12" t="s">
         <v>365</v>
       </c>
       <c r="G4"/>
@@ -22871,18 +22916,18 @@
       <c r="AMJ4"/>
     </row>
     <row r="5" spans="1:1024" ht="17.25" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>367</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="27" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="13"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
@@ -23903,18 +23948,18 @@
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" ht="34.9" customHeight="1">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>369</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="13"/>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
@@ -24935,16 +24980,16 @@
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="25" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="11" t="s">
         <v>373</v>
       </c>
       <c r="G7"/>
@@ -25967,18 +26012,18 @@
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" ht="20.25" customHeight="1">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="12" t="s">
         <v>377</v>
       </c>
       <c r="G8"/>
@@ -27001,16 +27046,16 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" ht="30" customHeight="1">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -28031,18 +28076,18 @@
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1024" ht="25.35" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="25" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="11" t="s">
         <v>383</v>
       </c>
       <c r="G10"/>
@@ -29065,18 +29110,18 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="24.6" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="26" t="s">
         <v>385</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="25" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="11" t="s">
         <v>353</v>
       </c>
       <c r="G11"/>
@@ -30099,18 +30144,18 @@
       <c r="AMJ11"/>
     </row>
     <row r="12" spans="1:1024" ht="35.65" customHeight="1">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="25" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="11" t="s">
         <v>353</v>
       </c>
       <c r="G12"/>
@@ -31133,16 +31178,16 @@
       <c r="AMJ12"/>
     </row>
     <row r="13" spans="1:1024" ht="18.95" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="28" t="s">
         <v>389</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="25" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11" t="s">
         <v>390</v>
       </c>
       <c r="G13"/>
@@ -32164,19 +32209,19 @@
       <c r="AMI13"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024" ht="18.2" customHeight="1">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:1024" ht="24.75" customHeight="1">
+      <c r="A14" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="28" t="s">
         <v>392</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="33" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="F14" s="28"/>
+      <c r="F14" s="13"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
@@ -33197,75 +33242,65 @@
       <c r="AMJ14"/>
     </row>
     <row r="15" spans="1:1024" ht="35.65" customHeight="1">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="26" t="s">
         <v>395</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="27" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:1024" ht="23.65" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="26" t="s">
         <v>397</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="27" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="F16" s="25"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="23.65" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="26" t="s">
         <v>400</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="27" t="s">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>403</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="F18" s="25"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="46.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="48.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
@@ -33275,6 +33310,16 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
print gridlines on PaediatricDosage
</commit_message>
<xml_diff>
--- a/PaediatricDosage.xlsx
+++ b/PaediatricDosage.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1818,13 +1818,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1835,35 +1844,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2162,7 +2162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
@@ -2189,123 +2189,123 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>60</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>80</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="26">
         <v>100</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="26">
         <v>120</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="26">
         <v>140</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="26">
         <v>150</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="26"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="26"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="26"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="26"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="26"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="25" t="s">
@@ -2381,21 +2381,21 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
@@ -2431,24 +2431,14 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="A17:B18"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="A33:C33"/>
@@ -2457,7 +2447,18 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2467,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView windowProtection="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2603,7 +2604,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B2"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2626,60 +2629,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="44.25" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="26"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="26"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="31" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
@@ -2735,29 +2738,29 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="29"/>
+      <c r="A22" s="32"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="31"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="30"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="21" t="s">
         <v>62</v>
       </c>
@@ -2778,30 +2781,31 @@
       <c r="A25" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:C5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:C8"/>
-    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:C8"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2828,38 +2832,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="19" t="s">
         <v>65</v>
       </c>
@@ -2874,31 +2878,31 @@
       <c r="B4" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="38" t="s">
         <v>385</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38" t="s">
         <v>386</v>
       </c>
-      <c r="F4" s="36"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="40"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
         <v>62</v>
       </c>
@@ -2919,11 +2923,11 @@
       <c r="A7" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="11" t="s">
         <v>399</v>
       </c>
@@ -2953,11 +2957,11 @@
       <c r="A9" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="11" t="s">
         <v>390</v>
       </c>
@@ -2985,11 +2989,11 @@
       <c r="A11" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="12" t="s">
         <v>392</v>
       </c>
@@ -3024,45 +3028,35 @@
         <v>89</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="39.75" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="10"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="B7:D7"/>
@@ -3071,7 +3065,18 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3098,31 +3103,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
@@ -3146,10 +3151,10 @@
       <c r="B4" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
         <v>97</v>
@@ -3159,10 +3164,10 @@
       <c r="A5" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="14" t="s">
         <v>100</v>
       </c>
@@ -3195,15 +3200,15 @@
       <c r="A7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="38" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="38"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="24">
       <c r="A8" s="11" t="s">
@@ -3223,11 +3228,11 @@
       <c r="A9" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="11" t="s">
         <v>398</v>
       </c>
@@ -3239,11 +3244,11 @@
       <c r="A10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="11" t="s">
         <v>399</v>
       </c>
@@ -3255,11 +3260,11 @@
       <c r="A11" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="11" t="s">
         <v>400</v>
       </c>
@@ -3271,11 +3276,11 @@
       <c r="A12" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="11" t="s">
         <v>400</v>
       </c>
@@ -3287,11 +3292,11 @@
       <c r="A13" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24" t="s">
         <v>126</v>
@@ -3301,23 +3306,23 @@
       <c r="A14" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>396</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6" ht="24">
       <c r="A15" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="14" t="s">
         <v>400</v>
       </c>
@@ -3329,11 +3334,11 @@
       <c r="A16" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="10" t="s">
         <v>133</v>
       </c>
@@ -3343,24 +3348,25 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3387,31 +3393,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
@@ -3432,11 +3438,11 @@
       <c r="A4" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="11" t="s">
         <v>402</v>
       </c>
@@ -3448,11 +3454,11 @@
       <c r="A5" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>140</v>
       </c>
@@ -3462,11 +3468,11 @@
       <c r="A6" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="11" t="s">
         <v>414</v>
       </c>
@@ -3478,11 +3484,11 @@
       <c r="A7" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="15" t="s">
         <v>146</v>
       </c>
@@ -3494,11 +3500,11 @@
       <c r="A8" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="11" t="s">
         <v>403</v>
       </c>
@@ -3510,11 +3516,11 @@
       <c r="A9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="12"/>
       <c r="F9" s="11" t="s">
         <v>415</v>
@@ -3524,11 +3530,11 @@
       <c r="A10" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="41" t="s">
         <v>417</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="12"/>
       <c r="F10" s="11" t="s">
         <v>416</v>
@@ -3538,11 +3544,11 @@
       <c r="A11" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="11" t="s">
         <v>400</v>
       </c>
@@ -3572,11 +3578,11 @@
       <c r="A13" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="10" t="s">
         <v>163</v>
       </c>
@@ -3588,11 +3594,11 @@
       <c r="A14" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="11" t="s">
         <v>399</v>
       </c>
@@ -3632,11 +3638,11 @@
       <c r="A17" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="10" t="s">
         <v>174</v>
       </c>
@@ -3646,11 +3652,11 @@
       <c r="A18" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="41" t="s">
         <v>420</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="11" t="s">
         <v>402</v>
       </c>
@@ -3660,11 +3666,11 @@
       <c r="A19" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="11" t="s">
         <v>402</v>
       </c>
@@ -3676,11 +3682,11 @@
       <c r="A20" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
       <c r="E20" s="11" t="s">
         <v>399</v>
       </c>
@@ -3688,16 +3694,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
@@ -3706,7 +3702,18 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3733,31 +3740,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
@@ -3781,10 +3788,10 @@
       <c r="B4" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="10" t="s">
         <v>185</v>
       </c>
@@ -3796,11 +3803,11 @@
       <c r="A5" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>421</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="11" t="s">
         <v>422</v>
       </c>
@@ -3812,11 +3819,11 @@
       <c r="A6" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="10" t="s">
         <v>191</v>
       </c>
@@ -3828,11 +3835,11 @@
       <c r="A7" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="43" t="s">
         <v>423</v>
       </c>
@@ -3842,11 +3849,11 @@
       <c r="A8" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="10" t="s">
         <v>133</v>
       </c>
@@ -3863,28 +3870,28 @@
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="41"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="19" t="s">
         <v>65</v>
       </c>
@@ -3896,11 +3903,11 @@
       <c r="A12" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="10" t="s">
         <v>202</v>
       </c>
@@ -3909,30 +3916,30 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="41" t="s">
         <v>204</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="36" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="38" t="s">
         <v>425</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="38" t="s">
         <v>424</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6" ht="52.5" customHeight="1">
       <c r="A15" s="10" t="s">
@@ -3941,10 +3948,10 @@
       <c r="B15" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="10" t="s">
         <v>174</v>
       </c>
@@ -3956,11 +3963,11 @@
       <c r="A16" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="11" t="s">
         <v>191</v>
       </c>
@@ -3972,11 +3979,11 @@
       <c r="A17" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="10" t="s">
         <v>191</v>
       </c>
@@ -3988,11 +3995,11 @@
       <c r="A18" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="38" t="s">
         <v>426</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="11" t="s">
         <v>218</v>
       </c>
@@ -4025,24 +4032,24 @@
       <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="40"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="41"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="19" t="s">
         <v>65</v>
       </c>
@@ -4054,11 +4061,11 @@
       <c r="A24" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
       <c r="E24" s="10" t="s">
         <v>222</v>
       </c>
@@ -4070,11 +4077,11 @@
       <c r="A25" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="10" t="s">
         <v>202</v>
       </c>
@@ -4084,38 +4091,39 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:D23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A19:F21"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A19:F21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:D23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4141,34 +4149,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="19" t="s">
         <v>65</v>
       </c>
@@ -4180,11 +4188,11 @@
       <c r="A4" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="11" t="s">
         <v>405</v>
       </c>
@@ -4196,11 +4204,11 @@
       <c r="A5" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>202</v>
       </c>
@@ -4235,24 +4243,24 @@
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="41"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="19" t="s">
         <v>65</v>
       </c>
@@ -4264,11 +4272,11 @@
       <c r="A11" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="10" t="s">
         <v>237</v>
       </c>
@@ -4280,11 +4288,11 @@
       <c r="A12" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="12"/>
       <c r="F12" s="10" t="s">
         <v>241</v>
@@ -4294,11 +4302,11 @@
       <c r="A13" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
@@ -4306,11 +4314,11 @@
       <c r="A14" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>427</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="11" t="s">
         <v>406</v>
       </c>
@@ -4322,11 +4330,11 @@
       <c r="A15" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="41" t="s">
         <v>247</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="11" t="s">
         <v>407</v>
       </c>
@@ -4336,11 +4344,11 @@
       <c r="A16" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="10" t="s">
         <v>174</v>
       </c>
@@ -4350,11 +4358,11 @@
       <c r="A17" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="12"/>
       <c r="F17" s="10" t="s">
         <v>252</v>
@@ -4364,11 +4372,11 @@
       <c r="A18" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="12"/>
       <c r="F18" s="11" t="s">
         <v>255</v>
@@ -4378,11 +4386,11 @@
       <c r="A19" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
@@ -4390,11 +4398,11 @@
       <c r="A20" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="41" t="s">
         <v>259</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
       <c r="E20" s="10" t="s">
         <v>260</v>
       </c>
@@ -4406,11 +4414,11 @@
       <c r="A21" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="38" t="s">
         <v>428</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="11" t="s">
         <v>408</v>
       </c>
@@ -4420,11 +4428,11 @@
       <c r="A22" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="10" t="s">
         <v>263</v>
       </c>
@@ -4434,21 +4442,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A6:F8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B16:D16"/>
@@ -4456,7 +4449,23 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A6:F8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4467,8 +4476,8 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6553,11 +6562,11 @@
       <c r="A3" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="11" t="s">
         <v>266</v>
       </c>
@@ -7587,11 +7596,11 @@
       <c r="A4" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="11" t="s">
         <v>400</v>
       </c>
@@ -8621,11 +8630,11 @@
       <c r="A5" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="11" t="s">
         <v>431</v>
       </c>
@@ -9655,11 +9664,11 @@
       <c r="A6" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>274</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="11" t="s">
         <v>409</v>
       </c>
@@ -10687,11 +10696,11 @@
       <c r="A7" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="12"/>
       <c r="F7" s="10" t="s">
         <v>66</v>
@@ -11719,11 +11728,11 @@
       <c r="A8" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="10" t="s">
         <v>279</v>
       </c>
@@ -12753,11 +12762,11 @@
       <c r="A9" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="41" t="s">
         <v>281</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="11" t="s">
         <v>410</v>
       </c>
@@ -13785,11 +13794,11 @@
       <c r="A10" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="38" t="s">
         <v>433</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="10" t="s">
         <v>283</v>
       </c>
@@ -14819,11 +14828,11 @@
       <c r="A11" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="12"/>
       <c r="F11" s="10" t="s">
         <v>287</v>
@@ -15851,11 +15860,11 @@
       <c r="A12" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="12"/>
       <c r="F12" s="10" t="s">
         <v>290</v>
@@ -16883,11 +16892,11 @@
       <c r="A13" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="10" t="s">
         <v>174</v>
       </c>
@@ -17917,11 +17926,11 @@
       <c r="A14" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="41" t="s">
         <v>295</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="12"/>
       <c r="F14" s="10" t="s">
         <v>296</v>
@@ -18949,11 +18958,11 @@
       <c r="A15" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
@@ -18961,9 +18970,9 @@
       <c r="A16" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
@@ -18971,11 +18980,11 @@
       <c r="A17" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="41" t="s">
         <v>301</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="10" t="s">
         <v>302</v>
       </c>
@@ -18987,11 +18996,11 @@
       <c r="A18" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
         <v>306</v>
@@ -19001,11 +19010,11 @@
       <c r="A19" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
@@ -19013,38 +19022,39 @@
       <c r="A20" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -21141,11 +21151,11 @@
       <c r="A3" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3"/>
@@ -22171,11 +22181,11 @@
       <c r="A4" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="11" t="s">
         <v>174</v>
       </c>
@@ -23205,11 +23215,11 @@
       <c r="A5" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="11" t="s">
         <v>202</v>
       </c>
@@ -24237,11 +24247,11 @@
       <c r="A6" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>319</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="11" t="s">
         <v>320</v>
       </c>
@@ -25269,11 +25279,11 @@
       <c r="A7" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="12"/>
       <c r="F7" s="10" t="s">
         <v>323</v>
@@ -26301,11 +26311,11 @@
       <c r="A8" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="10" t="s">
         <v>326</v>
       </c>
@@ -27335,11 +27345,11 @@
       <c r="A9" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9"/>
@@ -28365,11 +28375,11 @@
       <c r="A10" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="10" t="s">
         <v>332</v>
       </c>
@@ -29399,11 +29409,11 @@
       <c r="A11" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="11" t="s">
         <v>407</v>
       </c>
@@ -30433,11 +30443,11 @@
       <c r="A12" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="10" t="s">
         <v>222</v>
       </c>
@@ -31467,11 +31477,11 @@
       <c r="A13" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="41" t="s">
         <v>339</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="12"/>
       <c r="F13" s="10" t="s">
         <v>340</v>
@@ -32499,11 +32509,11 @@
       <c r="A14" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="41" t="s">
         <v>342</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="16" t="s">
         <v>411</v>
       </c>
@@ -33531,11 +33541,11 @@
       <c r="A15" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="11" t="s">
         <v>412</v>
       </c>
@@ -33545,11 +33555,11 @@
       <c r="A16" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="38" t="s">
         <v>346</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="11" t="s">
         <v>347</v>
       </c>
@@ -33559,11 +33569,11 @@
       <c r="A17" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="38" t="s">
         <v>349</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="11" t="s">
         <v>413</v>
       </c>
@@ -33573,11 +33583,11 @@
       <c r="A18" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="10" t="s">
         <v>222</v>
       </c>
@@ -33587,16 +33597,6 @@
     <row r="20" spans="1:6" ht="48.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
@@ -33606,7 +33606,18 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new file:   CUSTOM.DIC modified:   PaediatricDosage.xlsx
</commit_message>
<xml_diff>
--- a/PaediatricDosage.xlsx
+++ b/PaediatricDosage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Medical PC\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Medical PC\git\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -687,9 +687,6 @@
   </si>
   <si>
     <t>Ofloxacin</t>
-  </si>
-  <si>
-    <t>Pivmacillanum</t>
   </si>
   <si>
     <t>50 mg/kg/day, 6hourly, I/V, I/M or oral</t>
@@ -1647,6 +1644,9 @@
   <si>
     <t>5 mg/tsf,
 25 mg/amp</t>
+  </si>
+  <si>
+    <t>Pivmecillanam</t>
   </si>
 </sst>
 </file>
@@ -1818,13 +1818,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1835,35 +1844,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2189,123 +2189,123 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>60</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>80</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="26">
         <v>100</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="26">
         <v>120</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="26">
         <v>140</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="26">
         <v>150</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="26"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="26"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="26"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="26"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="26"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="25" t="s">
@@ -2358,7 +2358,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2381,21 +2381,21 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
@@ -2431,24 +2431,14 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="A17:B18"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="A33:C33"/>
@@ -2457,6 +2447,16 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2468,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+    <sheetView windowProtection="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2480,7 +2480,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="46" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" s="46"/>
     </row>
@@ -2490,42 +2490,42 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2533,39 +2533,39 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>366</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2573,31 +2573,31 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>375</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -2614,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
@@ -2629,68 +2629,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="A3" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="44.25" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="26"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="26"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="34"/>
+      <c r="A12" s="30"/>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
@@ -2739,36 +2739,36 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="29"/>
+      <c r="A22" s="32"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="31"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="30"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="21" t="s">
         <v>62</v>
       </c>
@@ -2789,29 +2789,29 @@
       <c r="A25" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26" t="s">
-        <v>383</v>
-      </c>
-      <c r="F25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="F25" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:C5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:C8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A1:F2"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A3:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:C8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A1:F2"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2825,7 +2825,7 @@
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2840,38 +2840,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="19" t="s">
         <v>65</v>
       </c>
@@ -2884,33 +2884,33 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>384</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38" t="s">
         <v>385</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36" t="s">
-        <v>386</v>
-      </c>
-      <c r="F4" s="36"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="40"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
         <v>62</v>
       </c>
@@ -2929,23 +2929,23 @@
     </row>
     <row r="7" spans="1:6" ht="54" customHeight="1">
       <c r="A7" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>387</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="36">
       <c r="A8" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>74</v>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>76</v>
@@ -2965,13 +2965,13 @@
       <c r="A9" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F9" s="12"/>
     </row>
@@ -2987,26 +2987,26 @@
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>392</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="182.25" customHeight="1">
@@ -3022,7 +3022,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24">
@@ -3036,45 +3036,35 @@
         <v>89</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="39.75" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="10"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="B7:D7"/>
@@ -3083,6 +3073,16 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3111,31 +3111,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
@@ -3159,10 +3159,10 @@
       <c r="B4" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
         <v>97</v>
@@ -3172,10 +3172,10 @@
       <c r="A5" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="14" t="s">
         <v>100</v>
       </c>
@@ -3192,13 +3192,13 @@
         <v>103</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>104</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>105</v>
@@ -3208,15 +3208,15 @@
       <c r="A7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="38" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="38"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="24">
       <c r="A8" s="11" t="s">
@@ -3236,13 +3236,13 @@
       <c r="A9" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>114</v>
@@ -3252,13 +3252,13 @@
       <c r="A10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>117</v>
@@ -3268,13 +3268,13 @@
       <c r="A11" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>120</v>
@@ -3284,13 +3284,13 @@
       <c r="A12" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>123</v>
@@ -3300,11 +3300,11 @@
       <c r="A13" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24" t="s">
         <v>126</v>
@@ -3314,25 +3314,25 @@
       <c r="A14" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>396</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="B14" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6" ht="24">
       <c r="A15" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>130</v>
@@ -3342,11 +3342,11 @@
       <c r="A16" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="10" t="s">
         <v>133</v>
       </c>
@@ -3356,23 +3356,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3384,9 +3384,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3401,31 +3401,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
@@ -3446,13 +3446,13 @@
       <c r="A4" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>137</v>
@@ -3462,11 +3462,11 @@
       <c r="A5" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>140</v>
       </c>
@@ -3476,13 +3476,13 @@
       <c r="A6" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>143</v>
@@ -3492,11 +3492,11 @@
       <c r="A7" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="15" t="s">
         <v>146</v>
       </c>
@@ -3508,13 +3508,13 @@
       <c r="A8" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>150</v>
@@ -3524,41 +3524,41 @@
       <c r="A9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="12"/>
       <c r="F9" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24">
       <c r="A10" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>417</v>
-      </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="B10" s="41" t="s">
+        <v>416</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="12"/>
       <c r="F10" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>156</v>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>160</v>
@@ -3586,29 +3586,29 @@
       <c r="A13" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="10" t="s">
         <v>163</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>164</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="16" spans="1:6" ht="29.25" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>169</v>
@@ -3646,11 +3646,11 @@
       <c r="A17" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="10" t="s">
         <v>174</v>
       </c>
@@ -3660,58 +3660,48 @@
       <c r="A18" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>420</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="B18" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="24">
       <c r="A19" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="24">
       <c r="A20" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
       <c r="E20" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
@@ -3720,6 +3710,16 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3748,31 +3748,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="A1" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
@@ -3791,77 +3791,77 @@
     </row>
     <row r="4" spans="1:6" ht="34.9" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.25" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="26.25" customHeight="1">
       <c r="A7" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="43" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="10" t="s">
         <v>133</v>
       </c>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="9" spans="1:6" ht="47.25" customHeight="1">
       <c r="A9" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -3878,28 +3878,28 @@
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="41"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="19" t="s">
         <v>65</v>
       </c>
@@ -3909,113 +3909,113 @@
     </row>
     <row r="12" spans="1:6" ht="45.75" customHeight="1">
       <c r="A12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="36" t="s">
-        <v>425</v>
-      </c>
-      <c r="F13" s="38"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="38" t="s">
+        <v>424</v>
+      </c>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="36" t="s">
-        <v>424</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="38" t="s">
+        <v>423</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6" ht="52.5" customHeight="1">
       <c r="A15" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="10" t="s">
         <v>174</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="27" customHeight="1">
       <c r="A16" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="38.25" customHeight="1">
       <c r="A17" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>215</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="45.75" customHeight="1">
       <c r="A18" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>426</v>
-      </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
@@ -4040,24 +4040,24 @@
       <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="40"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="41"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="19" t="s">
         <v>65</v>
       </c>
@@ -4067,69 +4067,69 @@
     </row>
     <row r="24" spans="1:6" ht="96">
       <c r="A24" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="33.75" customHeight="1">
       <c r="A25" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>225</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:D23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A19:F21"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A19:F21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:D23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4157,34 +4157,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="A1" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="19" t="s">
         <v>65</v>
       </c>
@@ -4194,39 +4194,39 @@
     </row>
     <row r="4" spans="1:6" ht="48.75" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="37.5" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>232</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1">
       <c r="A6" s="42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="42"/>
@@ -4251,24 +4251,24 @@
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="41"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="19" t="s">
         <v>65</v>
       </c>
@@ -4278,85 +4278,85 @@
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>237</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="49.5" customHeight="1">
       <c r="A12" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>240</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="12"/>
       <c r="F12" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="36.75" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" ht="40.5" customHeight="1">
       <c r="A14" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>426</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>427</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24">
       <c r="A15" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" ht="17.25" customHeight="1">
       <c r="A16" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="B16" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="10" t="s">
         <v>174</v>
       </c>
@@ -4364,107 +4364,92 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="B17" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="12"/>
       <c r="F17" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="37.5" customHeight="1">
       <c r="A18" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="12"/>
       <c r="F18" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>256</v>
       </c>
-      <c r="B19" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>258</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="10" t="s">
-        <v>260</v>
-      </c>
       <c r="F20" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>428</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
+        <v>260</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="87.75" customHeight="1">
       <c r="A22" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>428</v>
+      </c>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>429</v>
-      </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="11" t="s">
         <v>263</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>264</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A6:F8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B16:D16"/>
@@ -4472,6 +4457,21 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A6:F8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6568,18 +6568,18 @@
     </row>
     <row r="3" spans="1:1024" ht="37.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="B3" s="38" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>267</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -7602,18 +7602,18 @@
     </row>
     <row r="4" spans="1:1024" ht="27" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>429</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>268</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>269</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
@@ -8636,18 +8636,18 @@
     </row>
     <row r="5" spans="1:1024" ht="26.25" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -9670,15 +9670,15 @@
     </row>
     <row r="6" spans="1:1024" ht="64.5" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>274</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6"/>
@@ -10702,13 +10702,13 @@
     </row>
     <row r="7" spans="1:1024">
       <c r="A7" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="12"/>
       <c r="F7" s="10" t="s">
         <v>66</v>
@@ -11734,18 +11734,18 @@
     </row>
     <row r="8" spans="1:1024" ht="26.25" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>277</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="10" t="s">
-        <v>279</v>
-      </c>
       <c r="F8" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -12768,15 +12768,15 @@
     </row>
     <row r="9" spans="1:1024" ht="24">
       <c r="A9" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9"/>
@@ -13800,18 +13800,18 @@
     </row>
     <row r="10" spans="1:1024" ht="49.5" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>433</v>
-      </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>283</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>284</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -14834,16 +14834,16 @@
     </row>
     <row r="11" spans="1:1024" ht="26.25" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>286</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="12"/>
       <c r="F11" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -15866,16 +15866,16 @@
     </row>
     <row r="12" spans="1:1024" ht="37.5" customHeight="1">
       <c r="A12" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="12"/>
       <c r="F12" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -16898,18 +16898,18 @@
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="41" t="s">
         <v>291</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>292</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="10" t="s">
         <v>174</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -17932,16 +17932,16 @@
     </row>
     <row r="14" spans="1:1024">
       <c r="A14" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>295</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="12"/>
       <c r="F14" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -18964,103 +18964,103 @@
     </row>
     <row r="15" spans="1:1024" ht="26.25" customHeight="1">
       <c r="A15" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+        <v>298</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>302</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>304</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>305</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="38.25" customHeight="1">
       <c r="A19" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="B19" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>308</v>
-      </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="39" customHeight="1">
       <c r="A20" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B20" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>310</v>
-      </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -21157,13 +21157,13 @@
     </row>
     <row r="3" spans="1:1024" ht="25.35" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3"/>
@@ -22187,18 +22187,18 @@
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>314</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="11" t="s">
         <v>174</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
@@ -23221,15 +23221,15 @@
     </row>
     <row r="5" spans="1:1024" ht="17.25" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>316</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>317</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5"/>
@@ -24253,15 +24253,15 @@
     </row>
     <row r="6" spans="1:1024" ht="39" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>318</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="11" t="s">
         <v>319</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="11" t="s">
-        <v>320</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6"/>
@@ -25285,16 +25285,16 @@
     </row>
     <row r="7" spans="1:1024">
       <c r="A7" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="12"/>
       <c r="F7" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
@@ -26317,18 +26317,18 @@
     </row>
     <row r="8" spans="1:1024" ht="20.25" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>326</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>327</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -27351,13 +27351,13 @@
     </row>
     <row r="9" spans="1:1024" ht="30" customHeight="1">
       <c r="A9" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>328</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>329</v>
-      </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9"/>
@@ -28381,18 +28381,18 @@
     </row>
     <row r="10" spans="1:1024" ht="25.35" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B10" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>332</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>333</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -29415,18 +29415,18 @@
     </row>
     <row r="11" spans="1:1024" ht="24.6" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -30449,18 +30449,18 @@
     </row>
     <row r="12" spans="1:1024" ht="35.65" customHeight="1">
       <c r="A12" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>337</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -31483,16 +31483,16 @@
     </row>
     <row r="13" spans="1:1024" ht="18.95" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="41" t="s">
         <v>338</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>339</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="12"/>
       <c r="F13" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -32515,15 +32515,15 @@
     </row>
     <row r="14" spans="1:1024" ht="24.75" customHeight="1">
       <c r="A14" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>341</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14"/>
@@ -33547,57 +33547,57 @@
     </row>
     <row r="15" spans="1:1024" ht="35.65" customHeight="1">
       <c r="A15" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>344</v>
-      </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:1024" ht="23.65" customHeight="1">
       <c r="A16" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="11" t="s">
         <v>346</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="11" t="s">
-        <v>347</v>
       </c>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="23.65" customHeight="1">
       <c r="A17" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>350</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>351</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F18" s="10"/>
     </row>
@@ -33605,16 +33605,6 @@
     <row r="20" spans="1:6" ht="48.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
@@ -33624,6 +33614,16 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>